<commit_message>
INFOTILES: Added som instructions. Fixed bugs in Infotiles.bas Fixed tablename in excel file was infotile not infotiles
</commit_message>
<xml_diff>
--- a/infotiles/Install/1b LISA - table & field configuration/field config & options.xlsx
+++ b/infotiles/Install/1b LISA - table & field configuration/field config & options.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmd\Documents\GitHub\LimeBootstrapAppStore\infotiles\Install\1b LISA - table &amp; field configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AOL\Desktop\infotiles\Install\1b LISA - table &amp; field configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="15975" windowHeight="7200" activeTab="5"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="15975" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE_FIELDS_config" sheetId="5" r:id="rId1"/>
@@ -340,9 +340,6 @@
     <t>lbs.html</t>
   </si>
   <si>
-    <t>localname</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -352,9 +349,6 @@
     <t>Relation to [coworker]</t>
   </si>
   <si>
-    <t>Relation to [department]. NOT MANDATORY - functionality can be turned of in VBA</t>
-  </si>
-  <si>
     <t>COMMENT</t>
   </si>
   <si>
@@ -412,10 +406,16 @@
     <t>set Required = True + Add empty option</t>
   </si>
   <si>
-    <t>infotile</t>
-  </si>
-  <si>
     <t>InfoTile(s)</t>
+  </si>
+  <si>
+    <t>infotiles</t>
+  </si>
+  <si>
+    <t>Display name</t>
+  </si>
+  <si>
+    <t>Relation to [department] or office. NOT MANDATORY - functionality can be turned of in VBA</t>
   </si>
 </sst>
 </file>
@@ -874,8 +874,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,23 +901,23 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>103</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -934,7 +934,7 @@
         <v>98</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -951,7 +951,7 @@
         <v>82</v>
       </c>
       <c r="E8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -968,7 +968,7 @@
         <v>82</v>
       </c>
       <c r="E9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -985,7 +985,7 @@
         <v>82</v>
       </c>
       <c r="E10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1002,7 +1002,7 @@
         <v>82</v>
       </c>
       <c r="E11" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1019,7 +1019,7 @@
         <v>82</v>
       </c>
       <c r="E12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1027,16 +1027,16 @@
         <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D13" t="s">
         <v>99</v>
       </c>
       <c r="E13" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,7 +1053,7 @@
         <v>82</v>
       </c>
       <c r="E14" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,12 +1070,12 @@
         <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B16" t="s">
         <v>75</v>
@@ -1087,7 +1087,7 @@
         <v>82</v>
       </c>
       <c r="E16" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1104,7 +1104,7 @@
         <v>82</v>
       </c>
       <c r="E17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1123,13 +1123,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B19" t="s">
         <v>86</v>
       </c>
       <c r="C19" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D19" t="s">
         <v>82</v>
@@ -1163,7 +1163,7 @@
         <v>99</v>
       </c>
       <c r="E21" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1180,7 +1180,7 @@
         <v>82</v>
       </c>
       <c r="E22" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1211,7 +1211,7 @@
         <v>82</v>
       </c>
       <c r="E24" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1243,7 +1243,7 @@
         <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1318,10 +1318,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>
@@ -1566,7 +1566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R33" sqref="R33"/>
     </sheetView>
   </sheetViews>

</xml_diff>